<commit_message>
Nytt sätt att definiera tävlingsklasser
</commit_message>
<xml_diff>
--- a/mallar/Protokoll 2019 individuell klass_(mall).xlsx
+++ b/mallar/Protokoll 2019 individuell klass_(mall).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E90C3E-539E-4171-BE32-7F059AF7F786}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E872B15-D11A-4092-8B4F-2375A22DB7C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="9397" tabRatio="966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="197">
   <si>
     <t>Nation:</t>
   </si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>Från framlänges knästående till baklänges stående</t>
   </si>
   <si>
     <t>Framlänges kullerbytta från korset till sittande på halsen</t>
@@ -913,9 +910,6 @@
     <t>Grundövningar</t>
   </si>
   <si>
-    <t>Upphopp till armbågsstående</t>
-  </si>
-  <si>
     <t>Upphopp till baklänges axelstående</t>
   </si>
   <si>
@@ -950,6 +944,15 @@
   </si>
   <si>
     <t>Individuell minior grund D</t>
+  </si>
+  <si>
+    <t>Hopp från framlänges knästående till baklänges stående</t>
+  </si>
+  <si>
+    <t>Armbågsstående</t>
+  </si>
+  <si>
+    <t>Artistiskt</t>
   </si>
 </sst>
 </file>
@@ -1963,7 +1966,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="461">
+  <cellXfs count="463">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2881,7 +2884,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="167" fontId="1" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3011,6 +3013,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3505,8 +3516,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3517,23 +3528,23 @@
   <sheetData>
     <row r="1" spans="1:6" s="319" customFormat="1" ht="20.65" x14ac:dyDescent="0.6">
       <c r="A1" s="318" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="319" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="319" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:6" s="371" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="371" t="s">
-        <v>194</v>
+    <row r="5" spans="1:6" s="370" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="370" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -3541,18 +3552,18 @@
     <row r="8" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="319" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="319" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:6" s="283" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A11" s="283" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="208" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -3560,61 +3571,61 @@
     </row>
     <row r="15" spans="1:6" s="284" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A15" s="284" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="285" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" s="208"/>
       <c r="F16" s="285" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="D17" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" s="284"/>
       <c r="F17" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="G17" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="H17" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="208" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="280" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D18" s="280" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" s="287"/>
       <c r="F18" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="H18" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="G18" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="H18" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3629,26 +3640,26 @@
     </row>
     <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="208" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="280" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D20" s="280" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E20" s="287"/>
       <c r="F20" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="H20" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="G20" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="H20" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3663,26 +3674,26 @@
     </row>
     <row r="22" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="208" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D22" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E22" s="287"/>
       <c r="F22" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="H22" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="G22" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="H22" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3697,40 +3708,40 @@
     </row>
     <row r="24" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="208" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D24" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E24" s="287"/>
       <c r="F24" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G24" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="280" t="s">
         <v>122</v>
-      </c>
-      <c r="H24" s="280" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A25" s="332" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B25" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="C25" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="D25" s="280" t="s">
-        <v>119</v>
       </c>
       <c r="E25" s="286"/>
     </row>
@@ -3743,110 +3754,110 @@
     </row>
     <row r="27" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="208" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B27" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D27" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E27" s="287"/>
       <c r="F27" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="G27" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="H27" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A28" s="332" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B28" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C28" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="280" t="s">
         <v>122</v>
-      </c>
-      <c r="D28" s="280" t="s">
-        <v>123</v>
       </c>
       <c r="E28" s="286"/>
     </row>
     <row r="30" spans="1:9" s="284" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A30" s="284" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="285" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" s="208"/>
       <c r="F31" s="285" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="D32" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="284" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F32" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="G32" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="H32" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I32" s="284" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="208" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="H33" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="D33" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="E33" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="F33" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="H33" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="I33" s="280" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3862,31 +3873,31 @@
     </row>
     <row r="35" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="208" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="F35" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="H35" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="D35" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="E35" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="F35" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="G35" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="H35" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="I35" s="280" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3902,31 +3913,31 @@
     </row>
     <row r="37" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="208" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="E37" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="H37" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="E37" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="H37" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="I37" s="280" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3942,31 +3953,31 @@
     </row>
     <row r="39" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="208" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="282" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="280" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="D39" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="E39" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="F39" s="282" t="s">
-        <v>118</v>
-      </c>
-      <c r="G39" s="280" t="s">
+      <c r="H39" s="280" t="s">
         <v>122</v>
       </c>
-      <c r="H39" s="280" t="s">
-        <v>123</v>
-      </c>
       <c r="I39" s="280" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="25.5" x14ac:dyDescent="0.35">
@@ -3974,16 +3985,16 @@
         <v>159</v>
       </c>
       <c r="B40" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="D40" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="E40" s="280" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
@@ -3994,48 +4005,48 @@
     </row>
     <row r="42" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="208" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B42" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="E42" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="F42" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="H42" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="D42" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="E42" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="F42" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="G42" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="H42" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="I42" s="280" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A43" s="332" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B43" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="280" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="280" t="s">
-        <v>123</v>
-      </c>
       <c r="E43" s="280" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
@@ -4050,108 +4061,108 @@
       <c r="D45" s="286"/>
       <c r="E45" s="286"/>
     </row>
-    <row r="46" spans="1:14" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="284" t="s">
-        <v>124</v>
+    <row r="47" spans="1:14" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A47" s="284" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="285" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" s="208"/>
       <c r="F48" s="285" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J48" s="285" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K48" s="208"/>
       <c r="N48" s="285" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="D49" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E49" s="284"/>
       <c r="F49" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="G49" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="H49" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J49" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="K49" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="K49" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="L49" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M49" s="284"/>
       <c r="N49" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="O49" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="O49" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="P49" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="208" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B50" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" s="280" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D50" s="280" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E50" s="287"/>
       <c r="F50" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="H50" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="G50" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="H50" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="J50" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K50" s="280" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L50" s="280" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M50" s="287"/>
       <c r="N50" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O50" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="P50" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="O50" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="P50" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4173,45 +4184,45 @@
     </row>
     <row r="52" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="208" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52" s="280" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D52" s="280" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E52" s="287"/>
       <c r="F52" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="H52" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="G52" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="H52" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="J52" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K52" s="280" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L52" s="280" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M52" s="287"/>
       <c r="N52" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O52" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="P52" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="O52" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="P52" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4233,45 +4244,45 @@
     </row>
     <row r="54" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="208" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B54" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D54" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E54" s="287"/>
       <c r="F54" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="H54" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="G54" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="H54" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="J54" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K54" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L54" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M54" s="287"/>
       <c r="N54" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O54" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="P54" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="O54" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="P54" s="280" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4293,45 +4304,45 @@
     </row>
     <row r="56" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="208" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B56" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D56" s="280" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E56" s="287"/>
       <c r="F56" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="H56" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="J56" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="K56" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="L56" s="280" t="s">
         <v>118</v>
-      </c>
-      <c r="G56" s="280" t="s">
-        <v>122</v>
-      </c>
-      <c r="H56" s="280" t="s">
-        <v>123</v>
-      </c>
-      <c r="J56" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="K56" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="L56" s="280" t="s">
-        <v>119</v>
       </c>
       <c r="M56" s="287"/>
       <c r="N56" s="280" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O56" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="P56" s="280" t="s">
         <v>122</v>
-      </c>
-      <c r="P56" s="280" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.35">
@@ -4343,126 +4354,126 @@
     </row>
     <row r="59" spans="1:17" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A59" s="284" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="285" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C61" s="208"/>
       <c r="F61" s="285" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J61" s="285" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K61" s="208"/>
       <c r="N61" s="285" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="C62" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="D62" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E62" s="284" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F62" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="G62" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="H62" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I62" s="284" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J62" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="K62" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="K62" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="L62" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M62" s="284" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N62" s="284" t="s">
+        <v>113</v>
+      </c>
+      <c r="O62" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="O62" s="284" t="s">
-        <v>115</v>
-      </c>
       <c r="P62" s="284" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q62" s="284" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="208" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B63" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="F63" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G63" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="H63" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="D63" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="E63" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="F63" s="280" t="s">
+      <c r="I63" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="J63" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="K63" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="L63" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="M63" s="280" t="s">
+        <v>193</v>
+      </c>
+      <c r="N63" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O63" s="280" t="s">
+        <v>186</v>
+      </c>
+      <c r="P63" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="G63" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="H63" s="280" t="s">
-        <v>119</v>
-      </c>
-      <c r="I63" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="J63" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="K63" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="L63" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="M63" s="280" t="s">
-        <v>195</v>
-      </c>
-      <c r="N63" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="O63" s="280" t="s">
-        <v>188</v>
-      </c>
-      <c r="P63" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="Q63" s="280" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4486,55 +4497,55 @@
     </row>
     <row r="65" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="208" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B65" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="D65" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="E65" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="F65" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G65" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="H65" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="E65" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="F65" s="280" t="s">
+      <c r="I65" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="J65" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="K65" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="L65" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="M65" s="280" t="s">
+        <v>184</v>
+      </c>
+      <c r="N65" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O65" s="280" t="s">
+        <v>190</v>
+      </c>
+      <c r="P65" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="G65" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="H65" s="280" t="s">
-        <v>119</v>
-      </c>
-      <c r="I65" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="J65" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="K65" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="L65" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="M65" s="280" t="s">
-        <v>186</v>
-      </c>
-      <c r="N65" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="O65" s="280" t="s">
-        <v>192</v>
-      </c>
-      <c r="P65" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="Q65" s="280" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4558,55 +4569,55 @@
     </row>
     <row r="67" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="208" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B67" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="D67" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="F67" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G67" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="H67" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="D67" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="E67" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="F67" s="280" t="s">
+      <c r="I67" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="J67" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="K67" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="L67" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="M67" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="N67" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O67" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="P67" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="G67" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="H67" s="280" t="s">
-        <v>119</v>
-      </c>
-      <c r="I67" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="J67" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="K67" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="L67" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="M67" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="N67" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="O67" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="P67" s="280" t="s">
-        <v>119</v>
-      </c>
       <c r="Q67" s="280" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4630,60 +4641,60 @@
     </row>
     <row r="69" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="208" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" s="280" t="s">
+        <v>185</v>
+      </c>
+      <c r="F69" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="G69" s="280" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="280" t="s">
+      <c r="H69" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="I69" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="J69" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="K69" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="L69" s="280" t="s">
         <v>118</v>
       </c>
-      <c r="C69" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="D69" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="E69" s="280" t="s">
-        <v>187</v>
-      </c>
-      <c r="F69" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="G69" s="280" t="s">
+      <c r="M69" s="280" t="s">
+        <v>191</v>
+      </c>
+      <c r="N69" s="280" t="s">
+        <v>117</v>
+      </c>
+      <c r="O69" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="P69" s="280" t="s">
         <v>122</v>
       </c>
-      <c r="H69" s="280" t="s">
-        <v>123</v>
-      </c>
-      <c r="I69" s="280" t="s">
-        <v>122</v>
-      </c>
-      <c r="J69" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="K69" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="L69" s="280" t="s">
-        <v>119</v>
-      </c>
-      <c r="M69" s="280" t="s">
-        <v>193</v>
-      </c>
-      <c r="N69" s="280" t="s">
-        <v>118</v>
-      </c>
-      <c r="O69" s="280" t="s">
-        <v>122</v>
-      </c>
-      <c r="P69" s="280" t="s">
-        <v>123</v>
-      </c>
       <c r="Q69" s="280" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="322" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A73" s="321" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="284" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
@@ -4691,79 +4702,79 @@
         <v>65</v>
       </c>
       <c r="B74" s="326" t="s">
+        <v>113</v>
+      </c>
+      <c r="C74" s="326" t="s">
         <v>114</v>
       </c>
-      <c r="C74" s="326" t="s">
-        <v>115</v>
-      </c>
       <c r="D74" s="326" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E74" s="326" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F74" s="326" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="320" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="320" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="320" t="s">
+      <c r="C75" s="328" t="s">
+        <v>145</v>
+      </c>
+      <c r="D75" s="328" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" s="320" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="328" t="s">
-        <v>146</v>
-      </c>
-      <c r="D75" s="328" t="s">
-        <v>146</v>
-      </c>
-      <c r="E75" s="320" t="s">
+      <c r="F75" s="320" t="s">
         <v>135</v>
-      </c>
-      <c r="F75" s="320" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="320" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" s="320" t="s">
+        <v>133</v>
+      </c>
+      <c r="C76" s="320" t="s">
         <v>137</v>
       </c>
-      <c r="B76" s="320" t="s">
-        <v>134</v>
-      </c>
-      <c r="C76" s="320" t="s">
-        <v>138</v>
-      </c>
-      <c r="D76" s="320" t="s">
+      <c r="D76" s="328" t="s">
+        <v>196</v>
+      </c>
+      <c r="E76" s="320" t="s">
         <v>139</v>
       </c>
-      <c r="E76" s="320" t="s">
-        <v>140</v>
-      </c>
       <c r="F76" s="320" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="320" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B77" s="320" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C77" s="320" t="s">
-        <v>138</v>
-      </c>
-      <c r="D77" s="320" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="328" t="s">
+        <v>196</v>
+      </c>
+      <c r="E77" s="320" t="s">
         <v>139</v>
       </c>
-      <c r="E77" s="320" t="s">
-        <v>140</v>
-      </c>
       <c r="F77" s="320" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4773,7 +4784,7 @@
       <c r="D78" s="320"/>
       <c r="E78" s="320"/>
       <c r="F78" s="323" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4794,62 +4805,62 @@
     </row>
     <row r="82" spans="1:6" s="284" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A82" s="327" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B82" s="326" t="s">
+        <v>113</v>
+      </c>
+      <c r="C82" s="326" t="s">
         <v>114</v>
       </c>
-      <c r="C82" s="326" t="s">
-        <v>115</v>
-      </c>
       <c r="D82" s="326" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E82" s="326" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F82" s="326" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="320" t="s">
+        <v>132</v>
+      </c>
+      <c r="B83" s="320" t="s">
         <v>133</v>
       </c>
-      <c r="B83" s="320" t="s">
+      <c r="C83" s="328" t="s">
+        <v>145</v>
+      </c>
+      <c r="D83" s="328" t="s">
+        <v>145</v>
+      </c>
+      <c r="E83" s="320" t="s">
         <v>134</v>
       </c>
-      <c r="C83" s="328" t="s">
-        <v>146</v>
-      </c>
-      <c r="D83" s="328" t="s">
-        <v>146</v>
-      </c>
-      <c r="E83" s="320" t="s">
+      <c r="F83" s="320" t="s">
         <v>135</v>
-      </c>
-      <c r="F83" s="320" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="320" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="320" t="s">
+        <v>133</v>
+      </c>
+      <c r="C84" s="320" t="s">
         <v>137</v>
       </c>
-      <c r="B84" s="320" t="s">
-        <v>134</v>
-      </c>
-      <c r="C84" s="320" t="s">
+      <c r="D84" s="320" t="s">
         <v>138</v>
       </c>
-      <c r="D84" s="320" t="s">
+      <c r="E84" s="320" t="s">
         <v>139</v>
       </c>
-      <c r="E84" s="320" t="s">
-        <v>140</v>
-      </c>
       <c r="F84" s="320" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4859,12 +4870,13 @@
       <c r="D85" s="320"/>
       <c r="E85" s="320"/>
       <c r="F85" s="280" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="321" customFormat="1" ht="17.25" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4875,8 +4887,8 @@
   </sheetPr>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -4940,10 +4952,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -4957,10 +4969,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4985,10 +4997,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -5000,10 +5012,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -5015,10 +5027,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -5068,14 +5080,14 @@
       <c r="M14" s="52"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="430" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="431"/>
-      <c r="C15" s="431"/>
-      <c r="D15" s="431"/>
-      <c r="E15" s="431"/>
-      <c r="F15" s="432"/>
+      <c r="A15" s="432" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="433"/>
+      <c r="C15" s="433"/>
+      <c r="D15" s="433"/>
+      <c r="E15" s="433"/>
+      <c r="F15" s="434"/>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
       <c r="I15" s="14"/>
@@ -5084,14 +5096,14 @@
       <c r="L15" s="352"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="430" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="431"/>
-      <c r="C16" s="431"/>
-      <c r="D16" s="431"/>
-      <c r="E16" s="431"/>
-      <c r="F16" s="432"/>
+      <c r="A16" s="432" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="433"/>
+      <c r="C16" s="433"/>
+      <c r="D16" s="433"/>
+      <c r="E16" s="433"/>
+      <c r="F16" s="434"/>
       <c r="G16" s="59"/>
       <c r="H16" s="59"/>
       <c r="I16" s="14"/>
@@ -5101,7 +5113,7 @@
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="300" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B17" s="301"/>
       <c r="C17" s="301"/>
@@ -5117,7 +5129,7 @@
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="300" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B18" s="301"/>
       <c r="C18" s="301"/>
@@ -5133,7 +5145,7 @@
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="300" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" s="301"/>
       <c r="C19" s="301"/>
@@ -5152,27 +5164,27 @@
       <c r="L20" s="182"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="436" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="437"/>
-      <c r="C21" s="437"/>
-      <c r="D21" s="437"/>
-      <c r="E21" s="437"/>
-      <c r="F21" s="437"/>
-      <c r="G21" s="437"/>
-      <c r="H21" s="437"/>
-      <c r="I21" s="437"/>
+      <c r="A21" s="438" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="439"/>
+      <c r="C21" s="439"/>
+      <c r="D21" s="439"/>
+      <c r="E21" s="439"/>
+      <c r="F21" s="439"/>
+      <c r="G21" s="439"/>
+      <c r="H21" s="439"/>
+      <c r="I21" s="439"/>
       <c r="J21" s="181"/>
       <c r="K21" s="180"/>
       <c r="L21" s="10"/>
       <c r="R21" s="175"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="444" t="s">
+      <c r="A22" s="446" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="445"/>
+      <c r="B22" s="447"/>
       <c r="C22" s="179"/>
       <c r="D22" s="179"/>
       <c r="E22" s="179"/>
@@ -5187,18 +5199,18 @@
       <c r="R22" s="175"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="440" t="s">
+      <c r="A23" s="442" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="441"/>
+      <c r="B23" s="443"/>
       <c r="C23" s="362"/>
-      <c r="D23" s="438" t="s">
+      <c r="D23" s="440" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="439"/>
+      <c r="E23" s="441"/>
       <c r="F23" s="363"/>
       <c r="G23" s="308" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H23" s="309">
         <f>IFERROR(IF(ROUND(C23/F23,3)&gt;10,10,ROUND(C23/F23,3)),10)</f>
@@ -5208,7 +5220,7 @@
         <v>91</v>
       </c>
       <c r="J23" s="308" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K23" s="311">
         <f>10-H23</f>
@@ -5218,11 +5230,11 @@
       <c r="R23" s="175"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="442" t="s">
+      <c r="A24" s="444" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="443"/>
-      <c r="C24" s="443"/>
+      <c r="B24" s="445"/>
+      <c r="C24" s="445"/>
       <c r="D24" s="312"/>
       <c r="E24" s="312"/>
       <c r="F24" s="312"/>
@@ -5230,23 +5242,23 @@
       <c r="H24" s="312"/>
       <c r="I24" s="312"/>
       <c r="J24" s="313"/>
-      <c r="K24" s="372"/>
+      <c r="K24" s="371"/>
       <c r="R24" s="175"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="433" t="s">
+      <c r="A25" s="435" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="434"/>
-      <c r="C25" s="434"/>
-      <c r="D25" s="434"/>
-      <c r="E25" s="434"/>
-      <c r="F25" s="434"/>
-      <c r="G25" s="434"/>
-      <c r="H25" s="434"/>
-      <c r="I25" s="434"/>
-      <c r="J25" s="434"/>
-      <c r="K25" s="435"/>
+      <c r="B25" s="436"/>
+      <c r="C25" s="436"/>
+      <c r="D25" s="436"/>
+      <c r="E25" s="436"/>
+      <c r="F25" s="436"/>
+      <c r="G25" s="436"/>
+      <c r="H25" s="436"/>
+      <c r="I25" s="436"/>
+      <c r="J25" s="436"/>
+      <c r="K25" s="437"/>
       <c r="L25" s="11">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -5293,7 +5305,7 @@
     </row>
     <row r="28" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L28" s="168" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6005,17 +6017,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="151" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="452" t="s">
+      <c r="A2" s="454" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="452"/>
-      <c r="C2" s="452"/>
-      <c r="D2" s="452"/>
-      <c r="E2" s="452"/>
-      <c r="F2" s="452"/>
-      <c r="G2" s="452"/>
-      <c r="H2" s="452"/>
-      <c r="I2" s="452"/>
+      <c r="B2" s="454"/>
+      <c r="C2" s="454"/>
+      <c r="D2" s="454"/>
+      <c r="E2" s="454"/>
+      <c r="F2" s="454"/>
+      <c r="G2" s="454"/>
+      <c r="H2" s="454"/>
+      <c r="I2" s="454"/>
       <c r="J2" s="186"/>
       <c r="K2" s="186"/>
       <c r="L2" s="186"/>
@@ -6060,10 +6072,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="G5" s="185"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
@@ -6078,10 +6090,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="G6" s="184"/>
       <c r="H6" s="141"/>
       <c r="I6" s="17" t="s">
@@ -6112,10 +6124,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="G8" s="206"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -6130,10 +6142,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="G9" s="206"/>
       <c r="H9" s="183"/>
       <c r="I9" s="183"/>
@@ -6146,15 +6158,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="G10" s="206"/>
       <c r="H10" s="183"/>
       <c r="I10" s="183"/>
-      <c r="J10" s="448"/>
-      <c r="K10" s="448"/>
+      <c r="J10" s="450"/>
+      <c r="K10" s="450"/>
       <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6166,7 +6178,7 @@
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="158" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H12" s="205"/>
       <c r="I12" s="205"/>
@@ -6176,38 +6188,38 @@
     </row>
     <row r="13" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="341" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="342" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="342" t="s">
+      <c r="D13" s="455" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="453" t="s">
+      <c r="E13" s="456"/>
+      <c r="F13" s="342" t="s">
         <v>169</v>
       </c>
-      <c r="E13" s="454"/>
-      <c r="F13" s="342" t="s">
+      <c r="G13" s="342" t="s">
         <v>170</v>
       </c>
-      <c r="G13" s="342" t="s">
+      <c r="H13" s="343" t="s">
         <v>171</v>
       </c>
-      <c r="H13" s="343" t="s">
-        <v>172</v>
-      </c>
       <c r="I13" s="344" t="s">
-        <v>132</v>
-      </c>
-      <c r="J13" s="457" t="s">
-        <v>177</v>
-      </c>
-      <c r="K13" s="458"/>
+        <v>131</v>
+      </c>
+      <c r="J13" s="459" t="s">
+        <v>176</v>
+      </c>
+      <c r="K13" s="460"/>
       <c r="L13" s="205"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="364"/>
       <c r="C14" s="365"/>
-      <c r="D14" s="455"/>
-      <c r="E14" s="456"/>
+      <c r="D14" s="457"/>
+      <c r="E14" s="458"/>
       <c r="F14" s="365"/>
       <c r="G14" s="365"/>
       <c r="H14" s="366"/>
@@ -6215,11 +6227,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="459">
+      <c r="J14" s="461">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="460"/>
+      <c r="K14" s="462"/>
       <c r="L14" s="205"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6246,20 +6258,20 @@
     </row>
     <row r="17" spans="1:12" ht="61.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="333" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17" s="449" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="451" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="452"/>
+      <c r="D17" s="452"/>
+      <c r="E17" s="452"/>
+      <c r="F17" s="452"/>
+      <c r="G17" s="452"/>
+      <c r="H17" s="452"/>
+      <c r="I17" s="453"/>
+      <c r="J17" s="203" t="s">
         <v>173</v>
-      </c>
-      <c r="C17" s="450"/>
-      <c r="D17" s="450"/>
-      <c r="E17" s="450"/>
-      <c r="F17" s="450"/>
-      <c r="G17" s="450"/>
-      <c r="H17" s="450"/>
-      <c r="I17" s="451"/>
-      <c r="J17" s="203" t="s">
-        <v>174</v>
       </c>
       <c r="K17" s="314">
         <f>J14</f>
@@ -6271,21 +6283,21 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="446" t="s">
+      <c r="A18" s="448" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="425" t="s">
-        <v>175</v>
-      </c>
-      <c r="C18" s="426"/>
-      <c r="D18" s="426"/>
-      <c r="E18" s="426"/>
-      <c r="F18" s="426"/>
-      <c r="G18" s="426"/>
-      <c r="H18" s="426"/>
-      <c r="I18" s="426"/>
+      <c r="B18" s="427" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="428"/>
+      <c r="D18" s="428"/>
+      <c r="E18" s="428"/>
+      <c r="F18" s="428"/>
+      <c r="G18" s="428"/>
+      <c r="H18" s="428"/>
+      <c r="I18" s="428"/>
       <c r="J18" s="203" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K18" s="359"/>
       <c r="L18" s="202">
@@ -6294,19 +6306,19 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="447"/>
-      <c r="B19" s="427" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="428"/>
-      <c r="D19" s="428"/>
-      <c r="E19" s="428"/>
-      <c r="F19" s="428"/>
-      <c r="G19" s="428"/>
-      <c r="H19" s="428"/>
-      <c r="I19" s="428"/>
+      <c r="A19" s="449"/>
+      <c r="B19" s="429" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="430"/>
+      <c r="D19" s="430"/>
+      <c r="E19" s="430"/>
+      <c r="F19" s="430"/>
+      <c r="G19" s="430"/>
+      <c r="H19" s="430"/>
+      <c r="I19" s="430"/>
       <c r="J19" s="201" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K19" s="360"/>
       <c r="L19" s="200">
@@ -6533,10 +6545,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="388"/>
-      <c r="D4" s="388"/>
-      <c r="E4" s="388"/>
-      <c r="F4" s="388"/>
+      <c r="C4" s="387"/>
+      <c r="D4" s="387"/>
+      <c r="E4" s="387"/>
+      <c r="F4" s="387"/>
       <c r="H4" s="16"/>
       <c r="I4" s="17" t="s">
         <v>14</v>
@@ -6550,10 +6562,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6578,10 +6590,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="388"/>
-      <c r="D7" s="388"/>
-      <c r="E7" s="388"/>
-      <c r="F7" s="388"/>
+      <c r="C7" s="387"/>
+      <c r="D7" s="387"/>
+      <c r="E7" s="387"/>
+      <c r="F7" s="387"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -6593,10 +6605,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="388"/>
-      <c r="D8" s="388"/>
-      <c r="E8" s="388"/>
-      <c r="F8" s="388"/>
+      <c r="C8" s="387"/>
+      <c r="D8" s="387"/>
+      <c r="E8" s="387"/>
+      <c r="F8" s="387"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -6608,10 +6620,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -6645,215 +6657,215 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H12" s="389" t="s">
+      <c r="H12" s="388" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="390"/>
-      <c r="J12" s="391" t="s">
+      <c r="I12" s="389"/>
+      <c r="J12" s="390" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="391"/>
-      <c r="L12" s="391"/>
+      <c r="K12" s="390"/>
+      <c r="L12" s="390"/>
     </row>
     <row r="13" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="392" t="s">
+      <c r="A13" s="391" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="395" t="s">
+      <c r="B13" s="394" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="395" t="s">
+      <c r="C13" s="394" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="395"/>
-      <c r="E13" s="395"/>
-      <c r="F13" s="397" t="s">
+      <c r="D13" s="394"/>
+      <c r="E13" s="394"/>
+      <c r="F13" s="396" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="398"/>
+      <c r="G13" s="397"/>
       <c r="H13" s="21"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="379" t="s">
+      <c r="J13" s="378" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="381"/>
-      <c r="L13" s="375">
+      <c r="K13" s="380"/>
+      <c r="L13" s="374">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="393"/>
-      <c r="B14" s="396"/>
-      <c r="C14" s="396" t="s">
+      <c r="A14" s="392"/>
+      <c r="B14" s="395"/>
+      <c r="C14" s="395" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="396"/>
-      <c r="E14" s="396"/>
-      <c r="F14" s="399" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="400"/>
+      <c r="D14" s="395"/>
+      <c r="E14" s="395"/>
+      <c r="F14" s="398" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="399"/>
       <c r="H14" s="24"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="380"/>
-      <c r="K14" s="382"/>
-      <c r="L14" s="376"/>
+      <c r="J14" s="379"/>
+      <c r="K14" s="381"/>
+      <c r="L14" s="375"/>
     </row>
     <row r="15" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="393"/>
-      <c r="B15" s="396"/>
-      <c r="C15" s="396" t="s">
+      <c r="A15" s="392"/>
+      <c r="B15" s="395"/>
+      <c r="C15" s="395" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="396"/>
-      <c r="E15" s="396"/>
-      <c r="F15" s="399" t="s">
+      <c r="D15" s="395"/>
+      <c r="E15" s="395"/>
+      <c r="F15" s="398" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="400"/>
+      <c r="G15" s="399"/>
       <c r="H15" s="27"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="380"/>
-      <c r="K15" s="383"/>
-      <c r="L15" s="376"/>
+      <c r="J15" s="379"/>
+      <c r="K15" s="382"/>
+      <c r="L15" s="375"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="393"/>
-      <c r="B16" s="401" t="s">
+      <c r="A16" s="392"/>
+      <c r="B16" s="400" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="396" t="s">
+      <c r="C16" s="395" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="396"/>
-      <c r="E16" s="396"/>
-      <c r="F16" s="399" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" s="400"/>
+      <c r="D16" s="395"/>
+      <c r="E16" s="395"/>
+      <c r="F16" s="398" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="399"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="380" t="s">
+      <c r="J16" s="379" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="374"/>
-      <c r="L16" s="376">
+      <c r="K16" s="373"/>
+      <c r="L16" s="375">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="393"/>
-      <c r="B17" s="402"/>
-      <c r="C17" s="396" t="s">
+      <c r="A17" s="392"/>
+      <c r="B17" s="401"/>
+      <c r="C17" s="395" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="396"/>
-      <c r="E17" s="396"/>
-      <c r="F17" s="399" t="s">
+      <c r="D17" s="395"/>
+      <c r="E17" s="395"/>
+      <c r="F17" s="398" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="400"/>
+      <c r="G17" s="399"/>
       <c r="H17" s="24"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="380"/>
-      <c r="K17" s="374"/>
-      <c r="L17" s="376"/>
+      <c r="J17" s="379"/>
+      <c r="K17" s="373"/>
+      <c r="L17" s="375"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="394"/>
-      <c r="B18" s="403"/>
-      <c r="C18" s="405" t="s">
+      <c r="A18" s="393"/>
+      <c r="B18" s="402"/>
+      <c r="C18" s="404" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="405"/>
-      <c r="E18" s="405"/>
-      <c r="F18" s="386" t="s">
+      <c r="D18" s="404"/>
+      <c r="E18" s="404"/>
+      <c r="F18" s="385" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="387"/>
+      <c r="G18" s="386"/>
       <c r="H18" s="31"/>
       <c r="I18" s="32"/>
-      <c r="J18" s="404"/>
-      <c r="K18" s="384"/>
-      <c r="L18" s="385"/>
+      <c r="J18" s="403"/>
+      <c r="K18" s="383"/>
+      <c r="L18" s="384"/>
     </row>
     <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="392" t="s">
+      <c r="A19" s="391" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="409" t="s">
+      <c r="B19" s="408" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="395" t="s">
+      <c r="C19" s="394" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="395"/>
-      <c r="E19" s="395"/>
-      <c r="F19" s="412" t="s">
+      <c r="D19" s="394"/>
+      <c r="E19" s="394"/>
+      <c r="F19" s="411" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="413"/>
+      <c r="G19" s="412"/>
       <c r="H19" s="33"/>
       <c r="I19" s="34"/>
-      <c r="J19" s="379" t="s">
+      <c r="J19" s="378" t="s">
         <v>97</v>
       </c>
-      <c r="K19" s="373"/>
-      <c r="L19" s="375">
+      <c r="K19" s="372"/>
+      <c r="L19" s="374">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="393"/>
-      <c r="B20" s="410"/>
-      <c r="C20" s="396" t="s">
+      <c r="A20" s="392"/>
+      <c r="B20" s="409"/>
+      <c r="C20" s="395" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="396"/>
-      <c r="E20" s="396"/>
-      <c r="F20" s="399" t="s">
+      <c r="D20" s="395"/>
+      <c r="E20" s="395"/>
+      <c r="F20" s="398" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="400"/>
+      <c r="G20" s="399"/>
       <c r="H20" s="24"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="380"/>
-      <c r="K20" s="374"/>
-      <c r="L20" s="376"/>
+      <c r="J20" s="379"/>
+      <c r="K20" s="373"/>
+      <c r="L20" s="375"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="393"/>
-      <c r="B21" s="411"/>
-      <c r="C21" s="396" t="s">
+      <c r="A21" s="392"/>
+      <c r="B21" s="410"/>
+      <c r="C21" s="395" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="396"/>
-      <c r="E21" s="396"/>
-      <c r="F21" s="399" t="s">
+      <c r="D21" s="395"/>
+      <c r="E21" s="395"/>
+      <c r="F21" s="398" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="400"/>
+      <c r="G21" s="399"/>
       <c r="H21" s="27"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="380"/>
-      <c r="K21" s="374"/>
-      <c r="L21" s="376"/>
+      <c r="J21" s="379"/>
+      <c r="K21" s="373"/>
+      <c r="L21" s="375"/>
     </row>
     <row r="22" spans="1:12" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="394"/>
+      <c r="A22" s="393"/>
       <c r="B22" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="405"/>
-      <c r="D22" s="405"/>
-      <c r="E22" s="405"/>
-      <c r="F22" s="386" t="s">
+      <c r="C22" s="404"/>
+      <c r="D22" s="404"/>
+      <c r="E22" s="404"/>
+      <c r="F22" s="385" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="387"/>
+      <c r="G22" s="386"/>
       <c r="H22" s="36"/>
       <c r="I22" s="37"/>
       <c r="J22" s="38" t="s">
@@ -6872,15 +6884,15 @@
       <c r="B23" s="144" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="406" t="s">
+      <c r="C23" s="405" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="406"/>
-      <c r="E23" s="406"/>
-      <c r="F23" s="407" t="s">
+      <c r="D23" s="405"/>
+      <c r="E23" s="405"/>
+      <c r="F23" s="406" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="408"/>
+      <c r="G23" s="407"/>
       <c r="H23" s="40"/>
       <c r="I23" s="41"/>
       <c r="J23" s="42" t="s">
@@ -6919,11 +6931,11 @@
         <v>6</v>
       </c>
       <c r="J25" s="46"/>
-      <c r="K25" s="377">
+      <c r="K25" s="376">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="378"/>
+      <c r="L25" s="377"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K26" s="330"/>
@@ -7045,7 +7057,7 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="215" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="211"/>
       <c r="I3" s="212" t="s">
@@ -7077,10 +7089,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="218"/>
-      <c r="C5" s="414"/>
-      <c r="D5" s="414"/>
-      <c r="E5" s="414"/>
-      <c r="F5" s="414"/>
+      <c r="C5" s="413"/>
+      <c r="D5" s="413"/>
+      <c r="E5" s="413"/>
+      <c r="F5" s="413"/>
       <c r="H5" s="211"/>
       <c r="I5" s="212" t="s">
         <v>14</v>
@@ -7094,10 +7106,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="218"/>
-      <c r="C6" s="414"/>
-      <c r="D6" s="414"/>
-      <c r="E6" s="414"/>
-      <c r="F6" s="414"/>
+      <c r="C6" s="413"/>
+      <c r="D6" s="413"/>
+      <c r="E6" s="413"/>
+      <c r="F6" s="413"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7122,10 +7134,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="216"/>
-      <c r="C8" s="414"/>
-      <c r="D8" s="414"/>
-      <c r="E8" s="414"/>
-      <c r="F8" s="414"/>
+      <c r="C8" s="413"/>
+      <c r="D8" s="413"/>
+      <c r="E8" s="413"/>
+      <c r="F8" s="413"/>
       <c r="H8" s="220"/>
       <c r="I8" s="220"/>
       <c r="J8" s="220"/>
@@ -7137,10 +7149,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="218"/>
-      <c r="C9" s="414"/>
-      <c r="D9" s="414"/>
-      <c r="E9" s="414"/>
-      <c r="F9" s="414"/>
+      <c r="C9" s="413"/>
+      <c r="D9" s="413"/>
+      <c r="E9" s="413"/>
+      <c r="F9" s="413"/>
       <c r="H9" s="220"/>
       <c r="I9" s="220"/>
       <c r="J9" s="220"/>
@@ -7152,10 +7164,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="218"/>
-      <c r="C10" s="414"/>
-      <c r="D10" s="414"/>
-      <c r="E10" s="414"/>
-      <c r="F10" s="414"/>
+      <c r="C10" s="413"/>
+      <c r="D10" s="413"/>
+      <c r="E10" s="413"/>
+      <c r="F10" s="413"/>
       <c r="H10" s="220"/>
       <c r="I10" s="220"/>
       <c r="J10" s="220"/>
@@ -7473,8 +7485,8 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -7482,7 +7494,7 @@
     <col min="1" max="1" width="5.73046875" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.1328125" style="2"/>
     <col min="3" max="3" width="12.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.73046875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.265625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.19921875" style="2" customWidth="1"/>
     <col min="6" max="6" width="6.06640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.59765625" style="2" customWidth="1"/>
@@ -7510,7 +7522,7 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
@@ -7542,10 +7554,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -7559,10 +7571,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7587,10 +7599,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -7602,10 +7614,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7617,10 +7629,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -7780,13 +7792,13 @@
       <c r="L21" s="352"/>
     </row>
     <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="300" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="298"/>
-      <c r="C22" s="298"/>
-      <c r="D22" s="299"/>
-      <c r="E22" s="370"/>
+      <c r="A22" s="414" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="415"/>
+      <c r="C22" s="415"/>
+      <c r="D22" s="415"/>
+      <c r="E22" s="416"/>
       <c r="F22" s="59"/>
       <c r="G22" s="59"/>
       <c r="H22" s="59"/>
@@ -7921,7 +7933,8 @@
       <c r="L33" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A22:E22"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C6:F6"/>
@@ -7942,7 +7955,7 @@
   <sheetPr codeName="Blad5"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7978,7 +7991,7 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
@@ -8010,10 +8023,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -8027,10 +8040,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8055,10 +8068,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -8070,10 +8083,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -8085,10 +8098,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -8432,7 +8445,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="210" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H2" s="211"/>
       <c r="I2" s="212" t="s">
@@ -8476,10 +8489,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="218"/>
-      <c r="C5" s="414"/>
-      <c r="D5" s="414"/>
-      <c r="E5" s="414"/>
-      <c r="F5" s="414"/>
+      <c r="C5" s="413"/>
+      <c r="D5" s="413"/>
+      <c r="E5" s="413"/>
+      <c r="F5" s="413"/>
       <c r="H5" s="211"/>
       <c r="I5" s="212" t="s">
         <v>14</v>
@@ -8493,10 +8506,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="218"/>
-      <c r="C6" s="414"/>
-      <c r="D6" s="414"/>
-      <c r="E6" s="414"/>
-      <c r="F6" s="414"/>
+      <c r="C6" s="413"/>
+      <c r="D6" s="413"/>
+      <c r="E6" s="413"/>
+      <c r="F6" s="413"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8521,10 +8534,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="216"/>
-      <c r="C8" s="416"/>
-      <c r="D8" s="416"/>
-      <c r="E8" s="416"/>
-      <c r="F8" s="416"/>
+      <c r="C8" s="418"/>
+      <c r="D8" s="418"/>
+      <c r="E8" s="418"/>
+      <c r="F8" s="418"/>
       <c r="H8" s="220"/>
       <c r="I8" s="220"/>
       <c r="J8" s="220"/>
@@ -8536,10 +8549,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="218"/>
-      <c r="C9" s="414"/>
-      <c r="D9" s="414"/>
-      <c r="E9" s="414"/>
-      <c r="F9" s="414"/>
+      <c r="C9" s="413"/>
+      <c r="D9" s="413"/>
+      <c r="E9" s="413"/>
+      <c r="F9" s="413"/>
       <c r="H9" s="220"/>
       <c r="I9" s="220"/>
       <c r="J9" s="220"/>
@@ -8551,10 +8564,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="218"/>
-      <c r="C10" s="414"/>
-      <c r="D10" s="414"/>
-      <c r="E10" s="414"/>
-      <c r="F10" s="414"/>
+      <c r="C10" s="413"/>
+      <c r="D10" s="413"/>
+      <c r="E10" s="413"/>
+      <c r="F10" s="413"/>
       <c r="H10" s="220"/>
       <c r="I10" s="220"/>
       <c r="J10" s="220"/>
@@ -9556,7 +9569,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="76" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
@@ -9600,10 +9613,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -9617,10 +9630,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -9649,10 +9662,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -9664,10 +9677,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -9679,10 +9692,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -9810,7 +9823,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="80"/>
       <c r="D19" s="81"/>
@@ -9852,7 +9865,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" s="80"/>
       <c r="D21" s="81"/>
@@ -10053,7 +10066,7 @@
   <sheetPr codeName="Blad7"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -10707,7 +10720,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="76" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
@@ -10751,10 +10764,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10768,10 +10781,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -10800,10 +10813,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -10815,10 +10828,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -10830,10 +10843,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -10961,7 +10974,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="80"/>
       <c r="D19" s="81"/>
@@ -11003,7 +11016,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" s="80"/>
       <c r="D21" s="81"/>
@@ -11839,10 +11852,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="387"/>
+      <c r="D5" s="387"/>
+      <c r="E5" s="387"/>
+      <c r="F5" s="387"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -11856,10 +11869,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
+      <c r="E6" s="387"/>
+      <c r="F6" s="387"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -11888,10 +11901,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="415"/>
-      <c r="D8" s="415"/>
-      <c r="E8" s="415"/>
-      <c r="F8" s="415"/>
+      <c r="C8" s="417"/>
+      <c r="D8" s="417"/>
+      <c r="E8" s="417"/>
+      <c r="F8" s="417"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -11903,10 +11916,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="387"/>
+      <c r="D9" s="387"/>
+      <c r="E9" s="387"/>
+      <c r="F9" s="387"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -11918,10 +11931,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="387"/>
+      <c r="D10" s="387"/>
+      <c r="E10" s="387"/>
+      <c r="F10" s="387"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -11953,21 +11966,21 @@
       <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="417" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="419" t="s">
-        <v>151</v>
-      </c>
-      <c r="C14" s="420"/>
-      <c r="D14" s="420"/>
-      <c r="E14" s="420"/>
-      <c r="F14" s="420"/>
-      <c r="G14" s="420"/>
-      <c r="H14" s="420"/>
-      <c r="I14" s="421"/>
+      <c r="A14" s="419" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="421" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="422"/>
+      <c r="D14" s="422"/>
+      <c r="E14" s="422"/>
+      <c r="F14" s="422"/>
+      <c r="G14" s="422"/>
+      <c r="H14" s="422"/>
+      <c r="I14" s="423"/>
       <c r="J14" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K14" s="357"/>
       <c r="L14" s="334">
@@ -11977,19 +11990,19 @@
       <c r="M14" s="47"/>
     </row>
     <row r="15" spans="1:13" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="418"/>
-      <c r="B15" s="422" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="423"/>
-      <c r="D15" s="423"/>
-      <c r="E15" s="423"/>
-      <c r="F15" s="423"/>
-      <c r="G15" s="423"/>
-      <c r="H15" s="423"/>
-      <c r="I15" s="423"/>
+      <c r="A15" s="420"/>
+      <c r="B15" s="424" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="425"/>
+      <c r="D15" s="425"/>
+      <c r="E15" s="425"/>
+      <c r="F15" s="425"/>
+      <c r="G15" s="425"/>
+      <c r="H15" s="425"/>
+      <c r="I15" s="425"/>
       <c r="J15" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K15" s="358"/>
       <c r="L15" s="338">
@@ -11998,21 +12011,21 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="417" t="s">
-        <v>166</v>
-      </c>
-      <c r="B16" s="425" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="426"/>
-      <c r="D16" s="426"/>
-      <c r="E16" s="426"/>
-      <c r="F16" s="426"/>
-      <c r="G16" s="426"/>
-      <c r="H16" s="426"/>
-      <c r="I16" s="426"/>
+      <c r="A16" s="419" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="427" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="428"/>
+      <c r="D16" s="428"/>
+      <c r="E16" s="428"/>
+      <c r="F16" s="428"/>
+      <c r="G16" s="428"/>
+      <c r="H16" s="428"/>
+      <c r="I16" s="428"/>
       <c r="J16" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K16" s="359"/>
       <c r="L16" s="335">
@@ -12021,17 +12034,17 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="424"/>
-      <c r="B17" s="427" t="s">
-        <v>181</v>
-      </c>
-      <c r="C17" s="428"/>
-      <c r="D17" s="428"/>
-      <c r="E17" s="428"/>
-      <c r="F17" s="428"/>
-      <c r="G17" s="428"/>
-      <c r="H17" s="428"/>
-      <c r="I17" s="428"/>
+      <c r="A17" s="426"/>
+      <c r="B17" s="429" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="430"/>
+      <c r="D17" s="430"/>
+      <c r="E17" s="430"/>
+      <c r="F17" s="430"/>
+      <c r="G17" s="430"/>
+      <c r="H17" s="430"/>
+      <c r="I17" s="430"/>
       <c r="J17" s="26" t="s">
         <v>4</v>
       </c>
@@ -12042,19 +12055,19 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="418"/>
-      <c r="B18" s="429" t="s">
+      <c r="A18" s="420"/>
+      <c r="B18" s="431" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="423"/>
-      <c r="D18" s="423"/>
-      <c r="E18" s="423"/>
-      <c r="F18" s="423"/>
-      <c r="G18" s="423"/>
-      <c r="H18" s="423"/>
-      <c r="I18" s="423"/>
+      <c r="C18" s="425"/>
+      <c r="D18" s="425"/>
+      <c r="E18" s="425"/>
+      <c r="F18" s="425"/>
+      <c r="G18" s="425"/>
+      <c r="H18" s="425"/>
+      <c r="I18" s="425"/>
       <c r="J18" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K18" s="361"/>
       <c r="L18" s="337">
@@ -12280,12 +12293,12 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>

</xml_diff>